<commit_message>
- Sprites now display in the .Exe. Thank you, based Nora
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -94,15 +94,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4831,7 +4831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
@@ -4847,57 +4847,57 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
       <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -4924,8 +4924,8 @@
       <c r="R4" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="4"/>
-      <c r="U4" s="5"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="4"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C5">
@@ -4952,8 +4952,8 @@
       <c r="R5">
         <v>0.41753099999999999</v>
       </c>
-      <c r="T5" s="4"/>
-      <c r="U5" s="5"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="4"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C6">
@@ -4980,8 +4980,8 @@
       <c r="R6">
         <v>0.41688700000000001</v>
       </c>
-      <c r="T6" s="4"/>
-      <c r="U6" s="5"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="4"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C7">
@@ -5008,8 +5008,8 @@
       <c r="R7">
         <v>0.41300300000000001</v>
       </c>
-      <c r="T7" s="4"/>
-      <c r="U7" s="5"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="4"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C8">
@@ -5036,8 +5036,8 @@
       <c r="R8">
         <v>0.40138499999999999</v>
       </c>
-      <c r="T8" s="4"/>
-      <c r="U8" s="5"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="4"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C9">
@@ -5064,8 +5064,8 @@
       <c r="R9">
         <v>0.37036599999999997</v>
       </c>
-      <c r="T9" s="4"/>
-      <c r="U9" s="5"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="4"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C10">
@@ -5092,9 +5092,9 @@
       <c r="R10">
         <v>0.29793399999999998</v>
       </c>
-      <c r="T10" s="4"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="4"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C11">
@@ -5121,8 +5121,8 @@
       <c r="R11">
         <v>0.17697599999999999</v>
       </c>
-      <c r="T11" s="4"/>
-      <c r="U11" s="5"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="4"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C12">
@@ -5149,8 +5149,8 @@
       <c r="R12">
         <v>3.6357199999999999E-17</v>
       </c>
-      <c r="T12" s="4"/>
-      <c r="U12" s="5"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="4"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C13">
@@ -5177,8 +5177,8 @@
       <c r="R13">
         <v>-0.17697599999999999</v>
       </c>
-      <c r="T13" s="4"/>
-      <c r="U13" s="5"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="4"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C14">
@@ -5205,8 +5205,8 @@
       <c r="R14">
         <v>-0.29793399999999998</v>
       </c>
-      <c r="T14" s="4"/>
-      <c r="U14" s="5"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="4"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C15">
@@ -5233,8 +5233,8 @@
       <c r="R15">
         <v>-0.37036599999999997</v>
       </c>
-      <c r="T15" s="4"/>
-      <c r="U15" s="5"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="4"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C16">
@@ -5261,8 +5261,8 @@
       <c r="R16">
         <v>-0.40138499999999999</v>
       </c>
-      <c r="T16" s="4"/>
-      <c r="U16" s="5"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="4"/>
     </row>
     <row r="17" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C17">
@@ -5289,8 +5289,8 @@
       <c r="R17">
         <v>-0.41300300000000001</v>
       </c>
-      <c r="T17" s="6"/>
-      <c r="U17" s="8"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="7"/>
     </row>
     <row r="18" spans="3:21" x14ac:dyDescent="0.25">
       <c r="G18">

</xml_diff>